<commit_message>
Edit PM2.5 SRPbVT for nonroad
</commit_message>
<xml_diff>
--- a/InputData/trans/SRPbVT/Separately Regulated Pollutants by Vehicle Type.xlsx
+++ b/InputData/trans/SRPbVT/Separately Regulated Pollutants by Vehicle Type.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\trans\SRPbVT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-us\InputData\trans\SRPbVT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -208,7 +208,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,6 +220,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -248,18 +256,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -540,19 +551,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="101.140625" customWidth="1"/>
+    <col min="2" max="2" width="101.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -560,234 +573,237 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B17" s="3">
         <v>2018</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B22" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B24" s="3">
         <v>2009</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B26" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B26" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -799,15 +815,15 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -848,7 +864,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -889,7 +905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -930,7 +946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -971,7 +987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -991,7 +1007,7 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -1012,7 +1028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -1032,7 +1048,7 @@
         <v>1</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1053,7 +1069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>57</v>
       </c>

</xml_diff>